<commit_message>
🔄 synced local 'matlabfiles/' with remote 'matlabMfiles/'
</commit_message>
<xml_diff>
--- a/matlabfiles/capCorrispondenze/scienza.xlsx
+++ b/matlabfiles/capCorrispondenze/scienza.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\books\DataScienceWithMatlab\maltabMfiles\capCorrispondenze\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\books\DataScienceWithMatlab\EserciziRiepilogo\capCorrispondenze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C307AB30-049D-4ED0-8BB8-86348A2963AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9023AD-EB9D-4BD7-A0B5-A3AC3C35D3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,8 +177,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -194,7 +194,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="259080" y="335280"/>
-          <a:ext cx="8907780" cy="6484620"/>
+          <a:ext cx="9364980" cy="4194810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -643,167 +643,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>1) Calcolare la tabella di contingenza tra le variabili SCIENZA (righe) e TITOLO_STUDIO (colonne)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="it-IT"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>2) Calcolare la tabella delle frequenze teoriche nell'ipotesi di indipendenza tra le due variabili</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>3) Calcolare il valore del test chi quadrato ed il relativo p-value. Commentare il risultato ottenuto. Qual è il valore del test chi quadrato che ci attendiamo nell'ipotesi di indipendenza stocastica dei due fenomeni? </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>4) Calcolare</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> i profili riga. Dire qual è il profilo riga che si discosta di meno dalla media e qual è quello che si discosta maggiormente dalla media.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>5)  Calcolare l'inerzia totale </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>6) Discutere la quota di varianza spiegata dalle prime due dimensioni latenti</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="it-IT"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>7) Trovare le coordinate dei punti riga e colonna da rappresentare nel grafico. Commentare</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> il grafico che si ottiene.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT"/>
-            <a:t>8) Con riferimento</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="it-IT" baseline="0"/>
-            <a:t> alle righe, calcolare il contributo di ogni punto riga all'inerzia della prima dimensione e il contributo della prima dimensione all'inerzia dei punti riga. </a:t>
-          </a:r>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100"/>
-            <a:t>9) Calcolare</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" baseline="0"/>
-            <a:t> e commentare l'indice </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>gamma di Goodman e Kruskall</a:t>
-          </a:r>
           <a:endParaRPr lang="it-IT" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -10718,7 +10557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>

</xml_diff>